<commit_message>
Update data: Glamour (e-mail inquiry)
</commit_message>
<xml_diff>
--- a/df_followers.xlsx
+++ b/df_followers.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapto\OneDrive\Pulpit\Scraper 03.2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapto\OneDrive\Pulpit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D936DD-F28D-4D74-B3C1-5BAFF8225115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA11CF0-7862-46B7-B314-E0ABCE061BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -762,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1239,7 +1239,7 @@
         <v>399600</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -1250,13 +1250,13 @@
         <v>149000</v>
       </c>
       <c r="D17" s="5">
-        <v>3070</v>
+        <v>6210</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
       </c>
       <c r="F17" s="5">
-        <v>0</v>
+        <v>33500</v>
       </c>
       <c r="G17" s="5">
         <v>0</v>
@@ -1265,10 +1265,11 @@
         <v>92</v>
       </c>
       <c r="I17" s="5">
-        <v>337162</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>373802</v>
+      </c>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1297,7 +1298,7 @@
         <v>325414</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -1326,7 +1327,7 @@
         <v>318061</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>281000</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -1384,7 +1385,7 @@
         <v>259284</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -1413,7 +1414,7 @@
         <v>246058</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1442,7 +1443,7 @@
         <v>229013</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
@@ -1471,7 +1472,7 @@
         <v>210668</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
@@ -1500,7 +1501,7 @@
         <v>208981</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
@@ -1529,7 +1530,7 @@
         <v>208767</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>34</v>
       </c>
@@ -1558,7 +1559,7 @@
         <v>208625</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
@@ -1587,7 +1588,7 @@
         <v>200175</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -1616,7 +1617,7 @@
         <v>188015</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
@@ -1645,7 +1646,7 @@
         <v>183581</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
@@ -1674,7 +1675,7 @@
         <v>183548</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Add data Q2 2025
</commit_message>
<xml_diff>
--- a/df_followers.xlsx
+++ b/df_followers.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapto\OneDrive\Pulpit\Social Media Scraper 2025\clean_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6ED007-4F09-459E-AFEF-4A01C8C75C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
-  <si>
-    <t>Tytuł</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+  <si>
+    <t>Pismo</t>
   </si>
   <si>
     <t>Facebook</t>
@@ -46,12 +52,12 @@
     <t>Fakt Gazeta Codzienna</t>
   </si>
   <si>
+    <t>Super Express</t>
+  </si>
+  <si>
     <t>Gazeta Wyborcza</t>
   </si>
   <si>
-    <t>Super Express</t>
-  </si>
-  <si>
     <t>Przegląd Sportowy</t>
   </si>
   <si>
@@ -61,15 +67,15 @@
     <t>National Geographic Polska</t>
   </si>
   <si>
+    <t>Sieci</t>
+  </si>
+  <si>
     <t>Auto Świat Katalog</t>
   </si>
   <si>
     <t>Rzeczpospolita</t>
   </si>
   <si>
-    <t>Sieci</t>
-  </si>
-  <si>
     <t>Polityka</t>
   </si>
   <si>
@@ -109,15 +115,15 @@
     <t>Gazeta Wrocławska</t>
   </si>
   <si>
+    <t>Dziennik Zachodni</t>
+  </si>
+  <si>
     <t>Top Agrar Polska</t>
   </si>
   <si>
     <t>Gość Niedzielny</t>
   </si>
   <si>
-    <t>Dziennik Zachodni</t>
-  </si>
-  <si>
     <t>Tele Magazyn</t>
   </si>
   <si>
@@ -163,42 +169,42 @@
     <t>Weranda</t>
   </si>
   <si>
+    <t>Tygodnik Poradnik Rolniczy</t>
+  </si>
+  <si>
+    <t>Gazeta Polska</t>
+  </si>
+  <si>
+    <t>Wieści Rolnicze</t>
+  </si>
+  <si>
+    <t>Kurier Poranny</t>
+  </si>
+  <si>
+    <t>Express Ilustrowany</t>
+  </si>
+  <si>
     <t>Sprawny. Marketing</t>
   </si>
   <si>
-    <t>Tygodnik Poradnik Rolniczy</t>
-  </si>
-  <si>
-    <t>Gazeta Polska</t>
-  </si>
-  <si>
-    <t>Wieści Rolnicze</t>
-  </si>
-  <si>
-    <t>Kurier Poranny</t>
-  </si>
-  <si>
-    <t>Express Ilustrowany</t>
-  </si>
-  <si>
     <t>Parkiet Gazeta Giełdy</t>
   </si>
   <si>
+    <t>Dziennik Łódzki</t>
+  </si>
+  <si>
     <t>Głos - Dziennik Pomorza</t>
   </si>
   <si>
-    <t>Dziennik Łódzki</t>
-  </si>
-  <si>
     <t>Motor</t>
   </si>
   <si>
+    <t>Express Bydgoski</t>
+  </si>
+  <si>
     <t>Nowości - Dziennik Toruński</t>
   </si>
   <si>
-    <t>Express Bydgoski</t>
-  </si>
-  <si>
     <t>SENS</t>
   </si>
   <si>
@@ -208,81 +214,81 @@
     <t>Kurier Szczeciński</t>
   </si>
   <si>
+    <t>Twój Styl</t>
+  </si>
+  <si>
     <t>Wysokie Obcasy Extra</t>
   </si>
   <si>
     <t>Polska Metropolia Warszawska</t>
   </si>
   <si>
-    <t>Twój Styl</t>
+    <t>Ładny Dom</t>
+  </si>
+  <si>
+    <t>Świat Wiedzy</t>
+  </si>
+  <si>
+    <t>Gazeta Współczesna</t>
+  </si>
+  <si>
+    <t>Tele Tydzień</t>
+  </si>
+  <si>
+    <t>Dziennik Polski</t>
+  </si>
+  <si>
+    <t>Świat Seriali</t>
+  </si>
+  <si>
+    <t>DOZ Magazyn Dbam o Zdrowie</t>
+  </si>
+  <si>
+    <t>Świerszczyk</t>
+  </si>
+  <si>
+    <t>Pani</t>
+  </si>
+  <si>
+    <t>Tygodnik Angora</t>
+  </si>
+  <si>
+    <t>Automobilista</t>
+  </si>
+  <si>
+    <t>Wiedza i Życie</t>
+  </si>
+  <si>
+    <t>Świat Nauki</t>
+  </si>
+  <si>
+    <t>Wiadomości Rolnicze Polska</t>
+  </si>
+  <si>
+    <t>Dziennik Elbląski Tygodnik</t>
+  </si>
+  <si>
+    <t>Gazeta Podatkowa</t>
+  </si>
+  <si>
+    <t>Działkowiec</t>
+  </si>
+  <si>
+    <t>Newsweek Polska Historia</t>
+  </si>
+  <si>
+    <t>Mój Ogródek</t>
+  </si>
+  <si>
+    <t>Życie Bytomskie</t>
+  </si>
+  <si>
+    <t>Inżynier Budownictwa</t>
   </si>
   <si>
     <t>Vogue Polska</t>
   </si>
   <si>
-    <t>Ładny Dom</t>
-  </si>
-  <si>
-    <t>Świat Wiedzy</t>
-  </si>
-  <si>
-    <t>Gazeta Współczesna</t>
-  </si>
-  <si>
-    <t>Tele Tydzień</t>
-  </si>
-  <si>
-    <t>Świat Seriali</t>
-  </si>
-  <si>
-    <t>DOZ Magazyn Dbam o Zdrowie</t>
-  </si>
-  <si>
-    <t>Świerszczyk</t>
-  </si>
-  <si>
-    <t>Dziennik Polski</t>
-  </si>
-  <si>
-    <t>Tygodnik Angora</t>
-  </si>
-  <si>
-    <t>Automobilista</t>
-  </si>
-  <si>
-    <t>Pani</t>
-  </si>
-  <si>
-    <t>Wiedza i Życie</t>
-  </si>
-  <si>
-    <t>Świat Nauki</t>
-  </si>
-  <si>
-    <t>Wiadomości Rolnicze Polska</t>
-  </si>
-  <si>
-    <t>Gazeta Podatkowa</t>
-  </si>
-  <si>
-    <t>Działkowiec</t>
-  </si>
-  <si>
-    <t>Dziennik Elbląski Tygodnik</t>
-  </si>
-  <si>
-    <t>Mój Ogródek</t>
-  </si>
-  <si>
-    <t>Newsweek Polska Historia</t>
-  </si>
-  <si>
-    <t>Inżynier Budownictwa</t>
-  </si>
-  <si>
-    <t>Życie Bytomskie</t>
-  </si>
-  <si>
     <t>Przegląd</t>
   </si>
   <si>
@@ -295,18 +301,18 @@
     <t>Szef Kuchni Magazyn Branży Gastronomicznej</t>
   </si>
   <si>
+    <t>Ogólnopolskie Pismo Rynku FMCG Hurt &amp; Detal</t>
+  </si>
+  <si>
     <t>Miesięcznik Dealer</t>
   </si>
   <si>
-    <t>Ogólnopolskie Pismo Rynku FMCG Hurt &amp; Detal</t>
+    <t>Wróżka</t>
   </si>
   <si>
     <t>Poradnik Restauratora</t>
   </si>
   <si>
-    <t>Wróżka</t>
-  </si>
-  <si>
     <t>My Company Polska</t>
   </si>
   <si>
@@ -316,9 +322,6 @@
     <t>Mam Ogród</t>
   </si>
   <si>
-    <t>Sport</t>
-  </si>
-  <si>
     <t>Teraz Wilanów</t>
   </si>
   <si>
@@ -365,16 +368,13 @@
   </si>
   <si>
     <t>Olivia</t>
-  </si>
-  <si>
-    <t>Super Nowości</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,17 +433,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office 2007–2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -481,7 +489,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office 2007–2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -515,6 +523,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -549,9 +558,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office 2007–2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -724,14 +734,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I110"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
+    <col min="2" max="9" width="20.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -739,28 +755,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -768,387 +784,387 @@
         <v>1400000</v>
       </c>
       <c r="C2">
-        <v>77500</v>
+        <v>373000</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>79900</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>65400</v>
       </c>
       <c r="F2">
-        <v>91000</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>64600</v>
+        <v>187600</v>
       </c>
       <c r="H2">
-        <v>357000</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1990100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>2105900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3">
-        <v>798000</v>
+        <v>571000</v>
       </c>
       <c r="C3">
-        <v>195000</v>
+        <v>1160000</v>
       </c>
       <c r="D3">
-        <v>17955</v>
+        <v>26100</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>31600</v>
       </c>
       <c r="F3">
-        <v>16500</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>887600</v>
+        <v>159300</v>
       </c>
       <c r="H3">
-        <v>25500</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>1940555</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>1948000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4">
-        <v>546000</v>
+        <v>797000</v>
       </c>
       <c r="C4">
-        <v>16600</v>
+        <v>26900</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>199000</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>879000</v>
       </c>
       <c r="F4">
-        <v>46700</v>
+        <v>18018</v>
       </c>
       <c r="G4">
-        <v>30300</v>
+        <v>25900</v>
       </c>
       <c r="H4">
-        <v>1100000</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1739600</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>1945818</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5">
-        <v>923000</v>
+        <v>931000</v>
       </c>
       <c r="C5">
-        <v>82000</v>
+        <v>290000</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>82100</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>285800</v>
       </c>
       <c r="F5">
-        <v>85400</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>286100</v>
+        <v>89200</v>
       </c>
       <c r="H5">
-        <v>288000</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1664500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>1678100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
-        <v>518000</v>
+        <v>521000</v>
       </c>
       <c r="C6">
-        <v>63700</v>
+        <v>25100</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>64600</v>
       </c>
       <c r="E6">
+        <v>957200</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>811</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>963800</v>
-      </c>
-      <c r="H6">
-        <v>21200</v>
-      </c>
       <c r="I6">
-        <v>1567511</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>1568711</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7">
-        <v>455000</v>
+        <v>473000</v>
       </c>
       <c r="C7">
-        <v>131000</v>
+        <v>816000</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>133000</v>
       </c>
       <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>43</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>793000</v>
-      </c>
       <c r="I7">
-        <v>1379043</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>1422043</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8">
-        <v>583000</v>
+        <v>194000</v>
       </c>
       <c r="C8">
-        <v>27000</v>
+        <v>465000</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>86600</v>
       </c>
       <c r="F8">
-        <v>4876</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>95500</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>710376</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>745600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9">
-        <v>176000</v>
+        <v>587000</v>
       </c>
       <c r="C9">
-        <v>22500</v>
+        <v>95600</v>
       </c>
       <c r="D9">
-        <v>35664</v>
+        <v>26800</v>
       </c>
       <c r="E9">
-        <v>670</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>363600</v>
+        <v>4871</v>
       </c>
       <c r="H9">
-        <v>87800</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>686234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>714271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10">
-        <v>193000</v>
+        <v>184000</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>97300</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>24000</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>366400</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>35902</v>
       </c>
       <c r="G10">
-        <v>85800</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>399000</v>
+        <v>668</v>
       </c>
       <c r="I10">
-        <v>677800</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>708270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11">
-        <v>317000</v>
+        <v>318000</v>
       </c>
       <c r="C11">
-        <v>45800</v>
+        <v>10600</v>
       </c>
       <c r="D11">
-        <v>12195</v>
+        <v>47200</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>254400</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>12188</v>
       </c>
       <c r="G11">
-        <v>255600</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>8140</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>638735</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>642388</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12">
-        <v>290000</v>
+        <v>295000</v>
       </c>
       <c r="C12">
-        <v>154000</v>
+        <v>39400</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>156000</v>
       </c>
       <c r="E12">
-        <v>975</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>120200</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>122100</v>
       </c>
       <c r="H12">
-        <v>38700</v>
+        <v>976</v>
       </c>
       <c r="I12">
-        <v>603875</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>613476</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13">
-        <v>283000</v>
+        <v>286000</v>
       </c>
       <c r="C13">
-        <v>35700</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>220100</v>
+        <v>36100</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>47500</v>
       </c>
       <c r="F13">
-        <v>752</v>
+        <v>223005</v>
       </c>
       <c r="G13">
-        <v>46800</v>
+        <v>758</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>586352</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>593363</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14">
-        <v>354000</v>
+        <v>408000</v>
       </c>
       <c r="C14">
-        <v>75800</v>
+        <v>77800</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>84700</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>12800</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>18500</v>
       </c>
       <c r="H14">
-        <v>62200</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>504800</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>589000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
       <c r="B15">
-        <v>352000</v>
+        <v>353000</v>
       </c>
       <c r="C15">
-        <v>129000</v>
+        <v>6870</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>132000</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1160,71 +1176,71 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>6830</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>487830</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>491870</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16">
-        <v>256000</v>
+        <v>261000</v>
       </c>
       <c r="C16">
-        <v>127000</v>
+        <v>52300</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>128000</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>26700</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>30200</v>
       </c>
       <c r="H16">
-        <v>48700</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>458400</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>471500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
       <c r="B17">
-        <v>205000</v>
+        <v>212000</v>
       </c>
       <c r="C17">
-        <v>158000</v>
+        <v>16300</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>160000</v>
       </c>
       <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>60600</v>
+      </c>
+      <c r="H17">
         <v>92</v>
       </c>
-      <c r="F17">
-        <v>56400</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>14100</v>
-      </c>
       <c r="I17">
-        <v>433592</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>448992</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1232,33 +1248,33 @@
         <v>130000</v>
       </c>
       <c r="C18">
-        <v>7507</v>
+        <v>7120</v>
       </c>
       <c r="D18">
-        <v>116752</v>
+        <v>7591</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>69300</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>117691</v>
       </c>
       <c r="G18">
-        <v>68500</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>5870</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>328629</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>331702</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
       <c r="B19">
-        <v>310000</v>
+        <v>315000</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1279,10 +1295,10 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>310000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>315000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1290,463 +1306,463 @@
         <v>41000</v>
       </c>
       <c r="C20">
-        <v>3932</v>
+        <v>100000</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>3939</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>168300</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>165200</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>83300</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>293432</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>313239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
       <c r="B21">
-        <v>143000</v>
+        <v>147000</v>
       </c>
       <c r="C21">
-        <v>51800</v>
+        <v>12800</v>
       </c>
       <c r="D21">
-        <v>1240</v>
+        <v>53300</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>61500</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1310</v>
       </c>
       <c r="G21">
-        <v>61200</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>11800</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>269040</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>275910</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>29</v>
       </c>
       <c r="B22">
-        <v>101000</v>
+        <v>104000</v>
       </c>
       <c r="C22">
-        <v>8953</v>
+        <v>81700</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>9032</v>
       </c>
       <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>12900</v>
+      </c>
+      <c r="H22">
         <v>29700</v>
       </c>
-      <c r="F22">
-        <v>12600</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>81400</v>
-      </c>
       <c r="I22">
-        <v>233653</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>237332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
       <c r="B23">
-        <v>221000</v>
+        <v>228000</v>
       </c>
       <c r="C23">
-        <v>1234</v>
+        <v>1740</v>
       </c>
       <c r="D23">
-        <v>66</v>
+        <v>1257</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>510</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="G23">
-        <v>473</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>1730</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>224503</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>231575</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24">
-        <v>101000</v>
+        <v>205000</v>
       </c>
       <c r="C24">
-        <v>20500</v>
+        <v>8550</v>
       </c>
       <c r="D24">
-        <v>730</v>
+        <v>3242</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>11400</v>
       </c>
       <c r="F24">
-        <v>25900</v>
+        <v>603</v>
       </c>
       <c r="G24">
-        <v>4837</v>
+        <v>39</v>
       </c>
       <c r="H24">
-        <v>64800</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>217767</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>228834</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25">
-        <v>153000</v>
+        <v>103000</v>
       </c>
       <c r="C25">
-        <v>11100</v>
+        <v>65300</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>20700</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>4849</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>747</v>
       </c>
       <c r="G25">
-        <v>39100</v>
+        <v>26000</v>
       </c>
       <c r="H25">
-        <v>12000</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>215200</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>220596</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>33</v>
       </c>
       <c r="B26">
-        <v>189000</v>
+        <v>155000</v>
       </c>
       <c r="C26">
-        <v>2990</v>
+        <v>12800</v>
       </c>
       <c r="D26">
-        <v>596</v>
+        <v>11300</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>39100</v>
       </c>
       <c r="F26">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>11400</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>8480</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>212503</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>218200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>34</v>
       </c>
       <c r="B27">
-        <v>187000</v>
+        <v>188000</v>
       </c>
       <c r="C27">
-        <v>2640</v>
+        <v>21800</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>2637</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>168</v>
+        <v>0</v>
       </c>
       <c r="H27">
-        <v>21300</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>211108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>212607</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>35</v>
       </c>
       <c r="B28">
-        <v>181000</v>
+        <v>184000</v>
       </c>
       <c r="C28">
-        <v>1991</v>
+        <v>11100</v>
       </c>
       <c r="D28">
-        <v>453</v>
+        <v>2076</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>3114</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>457</v>
       </c>
       <c r="G28">
-        <v>3075</v>
+        <v>0</v>
       </c>
       <c r="H28">
-        <v>11000</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <v>197519</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>200747</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>36</v>
       </c>
       <c r="B29">
-        <v>176000</v>
+        <v>180000</v>
       </c>
       <c r="C29">
-        <v>1995</v>
+        <v>13200</v>
       </c>
       <c r="D29">
+        <v>2050</v>
+      </c>
+      <c r="E29">
+        <v>1297</v>
+      </c>
+      <c r="F29">
         <v>10</v>
       </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
       <c r="G29">
-        <v>1288</v>
+        <v>0</v>
       </c>
       <c r="H29">
-        <v>13100</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>192393</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>196557</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>37</v>
       </c>
       <c r="B30">
-        <v>170000</v>
+        <v>173000</v>
       </c>
       <c r="C30">
-        <v>2204</v>
+        <v>3930</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>2298</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>5416</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30">
-        <v>5456</v>
+        <v>0</v>
       </c>
       <c r="H30">
-        <v>3910</v>
+        <v>0</v>
       </c>
       <c r="I30">
-        <v>181570</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>184644</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>38</v>
       </c>
       <c r="B31">
-        <v>168000</v>
+        <v>172000</v>
       </c>
       <c r="C31">
-        <v>4678</v>
+        <v>431</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>4808</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>6669</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
       <c r="G31">
-        <v>6673</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>275</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>179626</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>183908</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>39</v>
       </c>
       <c r="B32">
-        <v>146000</v>
+        <v>158000</v>
       </c>
       <c r="C32">
-        <v>2645</v>
+        <v>3530</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>2771</v>
       </c>
       <c r="E32">
-        <v>152</v>
+        <v>12500</v>
       </c>
       <c r="F32">
         <v>0</v>
       </c>
       <c r="G32">
-        <v>12300</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>3470</v>
+        <v>151</v>
       </c>
       <c r="I32">
-        <v>164567</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>176952</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>40</v>
       </c>
       <c r="B33">
-        <v>146000</v>
+        <v>149000</v>
       </c>
       <c r="C33">
+        <v>350</v>
+      </c>
+      <c r="D33">
         <v>10100</v>
       </c>
-      <c r="D33">
+      <c r="E33">
+        <v>5644</v>
+      </c>
+      <c r="F33">
         <v>40</v>
       </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
       <c r="G33">
-        <v>5646</v>
+        <v>0</v>
       </c>
       <c r="H33">
-        <v>344</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>162130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>165134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>41</v>
       </c>
       <c r="B34">
-        <v>128000</v>
+        <v>130000</v>
       </c>
       <c r="C34">
-        <v>7444</v>
+        <v>19700</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>7460</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>4251</v>
       </c>
       <c r="F34">
-        <v>2772</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>4229</v>
+        <v>2943</v>
       </c>
       <c r="H34">
-        <v>19000</v>
+        <v>0</v>
       </c>
       <c r="I34">
-        <v>161445</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>164354</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>42</v>
       </c>
       <c r="B35">
-        <v>143000</v>
+        <v>146000</v>
       </c>
       <c r="C35">
-        <v>4704</v>
+        <v>9180</v>
       </c>
       <c r="D35">
-        <v>69</v>
+        <v>4743</v>
       </c>
       <c r="E35">
+        <v>3384</v>
+      </c>
+      <c r="F35">
+        <v>72</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
         <v>47</v>
       </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>3388</v>
-      </c>
-      <c r="H35">
-        <v>9140</v>
-      </c>
       <c r="I35">
-        <v>160348</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>163426</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -1754,10 +1770,10 @@
         <v>157000</v>
       </c>
       <c r="C36">
-        <v>2658</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>2687</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1772,53 +1788,53 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <v>159658</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>159687</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>44</v>
       </c>
       <c r="B37">
-        <v>136000</v>
+        <v>140000</v>
       </c>
       <c r="C37">
-        <v>7037</v>
+        <v>75</v>
       </c>
       <c r="D37">
-        <v>84</v>
+        <v>7200</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>8717</v>
       </c>
       <c r="F37">
+        <v>85</v>
+      </c>
+      <c r="G37">
         <v>16</v>
       </c>
-      <c r="G37">
-        <v>8705</v>
-      </c>
       <c r="H37">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="I37">
-        <v>151914</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>156093</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>45</v>
       </c>
       <c r="B38">
-        <v>61000</v>
+        <v>62000</v>
       </c>
       <c r="C38">
-        <v>46200</v>
+        <v>39400</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>46800</v>
       </c>
       <c r="E38">
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1827,42 +1843,42 @@
         <v>0</v>
       </c>
       <c r="H38">
-        <v>38700</v>
+        <v>167</v>
       </c>
       <c r="I38">
-        <v>146066</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>148367</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>46</v>
       </c>
       <c r="B39">
-        <v>134000</v>
+        <v>138000</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>6440</v>
       </c>
       <c r="D39">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>3447</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="G39">
-        <v>3476</v>
+        <v>0</v>
       </c>
       <c r="H39">
-        <v>6390</v>
+        <v>0</v>
       </c>
       <c r="I39">
-        <v>143929</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <v>147978</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1870,28 +1886,28 @@
         <v>23000</v>
       </c>
       <c r="C40">
-        <v>4379</v>
+        <v>13800</v>
       </c>
       <c r="D40">
-        <v>60820</v>
+        <v>4417</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>43400</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>60907</v>
       </c>
       <c r="G40">
-        <v>41800</v>
+        <v>0</v>
       </c>
       <c r="H40">
-        <v>9800</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <v>139799</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>145524</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -1899,97 +1915,97 @@
         <v>98000</v>
       </c>
       <c r="C41">
-        <v>39200</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
         <v>1400</v>
       </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
       <c r="I41">
-        <v>138600</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+        <v>139400</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>49</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>96000</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>18000</v>
       </c>
       <c r="D42">
-        <v>80676</v>
+        <v>9054</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>1837</v>
       </c>
       <c r="F42">
-        <v>16400</v>
+        <v>119</v>
       </c>
       <c r="G42">
-        <v>8061</v>
+        <v>0</v>
       </c>
       <c r="H42">
-        <v>19700</v>
+        <v>0</v>
       </c>
       <c r="I42">
-        <v>124837</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>125010</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>50</v>
       </c>
       <c r="B43">
-        <v>90000</v>
+        <v>38000</v>
       </c>
       <c r="C43">
-        <v>9060</v>
+        <v>39600</v>
       </c>
       <c r="D43">
-        <v>118</v>
+        <v>7140</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>28500</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>1841</v>
+        <v>0</v>
       </c>
       <c r="H43">
-        <v>17800</v>
+        <v>0</v>
       </c>
       <c r="I43">
-        <v>118819</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>113240</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>51</v>
       </c>
       <c r="B44">
-        <v>38000</v>
+        <v>35000</v>
       </c>
       <c r="C44">
-        <v>6461</v>
+        <v>65700</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1736</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1998,82 +2014,82 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <v>28200</v>
+        <v>9828</v>
       </c>
       <c r="H44">
-        <v>39300</v>
+        <v>0</v>
       </c>
       <c r="I44">
-        <v>111961</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>112264</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>52</v>
       </c>
       <c r="B45">
-        <v>34000</v>
+        <v>97000</v>
       </c>
       <c r="C45">
-        <v>1708</v>
+        <v>4220</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>4125</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>3238</v>
       </c>
       <c r="F45">
-        <v>8077</v>
+        <v>0</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45">
-        <v>64000</v>
+        <v>0</v>
       </c>
       <c r="I45">
-        <v>107785</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>108583</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>53</v>
       </c>
       <c r="B46">
-        <v>96000</v>
+        <v>97000</v>
       </c>
       <c r="C46">
-        <v>4118</v>
+        <v>2550</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>3039</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>1430</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
       <c r="G46">
-        <v>3235</v>
+        <v>0</v>
       </c>
       <c r="H46">
-        <v>4200</v>
+        <v>0</v>
       </c>
       <c r="I46">
-        <v>107553</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+        <v>104019</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>54</v>
       </c>
       <c r="B47">
-        <v>92000</v>
+        <v>0</v>
       </c>
       <c r="C47">
-        <v>3041</v>
+        <v>0</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -2082,106 +2098,106 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>83067</v>
       </c>
       <c r="G47">
-        <v>1430</v>
+        <v>16500</v>
       </c>
       <c r="H47">
-        <v>2560</v>
+        <v>0</v>
       </c>
       <c r="I47">
-        <v>99031</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>99567</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>55</v>
       </c>
       <c r="B48">
-        <v>45000</v>
+        <v>44000</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>22400</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>27300</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
       <c r="G48">
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="H48">
-        <v>22000</v>
+        <v>0</v>
       </c>
       <c r="I48">
-        <v>94000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>93700</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>56</v>
       </c>
       <c r="B49">
-        <v>77000</v>
+        <v>76000</v>
       </c>
       <c r="C49">
-        <v>1425</v>
+        <v>4790</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>2780</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>4773</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G49">
-        <v>1840</v>
+        <v>0</v>
       </c>
       <c r="H49">
-        <v>6220</v>
+        <v>0</v>
       </c>
       <c r="I49">
-        <v>86485</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+        <v>88345</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>57</v>
       </c>
       <c r="B50">
-        <v>74000</v>
+        <v>78000</v>
       </c>
       <c r="C50">
-        <v>2686</v>
+        <v>6240</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>1443</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>1833</v>
       </c>
       <c r="F50">
         <v>0</v>
       </c>
       <c r="G50">
-        <v>4818</v>
+        <v>0</v>
       </c>
       <c r="H50">
-        <v>4780</v>
+        <v>0</v>
       </c>
       <c r="I50">
-        <v>86286</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>87516</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -2210,7 +2226,7 @@
         <v>78000</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -2218,68 +2234,68 @@
         <v>71000</v>
       </c>
       <c r="C52">
-        <v>674</v>
+        <v>2780</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>3099</v>
       </c>
       <c r="F52">
         <v>0</v>
       </c>
       <c r="G52">
-        <v>2161</v>
+        <v>0</v>
       </c>
       <c r="H52">
-        <v>1280</v>
+        <v>0</v>
       </c>
       <c r="I52">
-        <v>75115</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>76879</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>60</v>
       </c>
       <c r="B53">
-        <v>68000</v>
+        <v>71000</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1290</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>719</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>2154</v>
       </c>
       <c r="F53">
         <v>0</v>
       </c>
       <c r="G53">
-        <v>3130</v>
+        <v>0</v>
       </c>
       <c r="H53">
-        <v>2770</v>
+        <v>0</v>
       </c>
       <c r="I53">
-        <v>73900</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>75163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>61</v>
       </c>
       <c r="B54">
-        <v>71000</v>
+        <v>72000</v>
       </c>
       <c r="C54">
-        <v>1397</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>1513</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -2294,79 +2310,79 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <v>72397</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>73513</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>62</v>
       </c>
       <c r="B55">
-        <v>34000</v>
+        <v>35000</v>
       </c>
       <c r="C55">
-        <v>27800</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>28200</v>
       </c>
       <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
         <v>10000</v>
       </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
       <c r="I55">
-        <v>71800</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>73200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>63</v>
       </c>
       <c r="B56">
-        <v>48000</v>
+        <v>50000</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>3130</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>2778</v>
       </c>
       <c r="F56">
-        <v>1115</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>2785</v>
+        <v>1120</v>
       </c>
       <c r="H56">
-        <v>3050</v>
+        <v>0</v>
       </c>
       <c r="I56">
-        <v>54950</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+        <v>57028</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>64</v>
       </c>
       <c r="B57">
-        <v>22000</v>
+        <v>25000</v>
       </c>
       <c r="C57">
-        <v>30800</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>27700</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -2375,27 +2391,27 @@
         <v>0</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>802</v>
       </c>
       <c r="H57">
         <v>0</v>
       </c>
       <c r="I57">
-        <v>52800</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>53502</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>65</v>
       </c>
       <c r="B58">
-        <v>52000</v>
+        <v>22000</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>30700</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -2410,18 +2426,18 @@
         <v>0</v>
       </c>
       <c r="I58">
-        <v>52000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>52700</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>66</v>
       </c>
       <c r="B59">
-        <v>21000</v>
+        <v>52000</v>
       </c>
       <c r="C59">
-        <v>26100</v>
+        <v>0</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2430,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>805</v>
+        <v>0</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2439,47 +2455,47 @@
         <v>0</v>
       </c>
       <c r="I59">
-        <v>47905</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>67</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>43000</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60">
-        <v>16800</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>1604</v>
+        <v>0</v>
       </c>
       <c r="H60">
-        <v>28500</v>
+        <v>0</v>
       </c>
       <c r="I60">
-        <v>46904</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>43336</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>68</v>
       </c>
       <c r="B61">
-        <v>43000</v>
+        <v>40000</v>
       </c>
       <c r="C61">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2497,24 +2513,24 @@
         <v>0</v>
       </c>
       <c r="I61">
-        <v>43330</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>69</v>
       </c>
       <c r="B62">
-        <v>40000</v>
+        <v>37000</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>710</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>2144</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -2526,21 +2542,21 @@
         <v>0</v>
       </c>
       <c r="I62">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+        <v>39869</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>70</v>
       </c>
       <c r="B63">
-        <v>36000</v>
+        <v>35000</v>
       </c>
       <c r="C63">
-        <v>710</v>
+        <v>0</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>4719</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -2549,33 +2565,33 @@
         <v>0</v>
       </c>
       <c r="G63">
-        <v>2142</v>
+        <v>0</v>
       </c>
       <c r="H63">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I63">
-        <v>38867</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+        <v>39719</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>71</v>
       </c>
       <c r="B64">
-        <v>34000</v>
+        <v>37000</v>
       </c>
       <c r="C64">
-        <v>4743</v>
+        <v>0</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>1941</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -2584,10 +2600,10 @@
         <v>0</v>
       </c>
       <c r="I64">
-        <v>38743</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>38973</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -2595,10 +2611,10 @@
         <v>37000</v>
       </c>
       <c r="C65">
-        <v>991</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -2613,10 +2629,10 @@
         <v>0</v>
       </c>
       <c r="I65">
-        <v>37991</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>38000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -2624,10 +2640,10 @@
         <v>36000</v>
       </c>
       <c r="C66">
-        <v>684</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>689</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -2642,21 +2658,21 @@
         <v>0</v>
       </c>
       <c r="I66">
-        <v>36684</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>36689</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>74</v>
       </c>
       <c r="B67">
-        <v>31000</v>
+        <v>32000</v>
       </c>
       <c r="C67">
-        <v>3549</v>
+        <v>606</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>3760</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -2668,24 +2684,24 @@
         <v>0</v>
       </c>
       <c r="H67">
-        <v>597</v>
+        <v>0</v>
       </c>
       <c r="I67">
-        <v>35146</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>36366</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>75</v>
       </c>
       <c r="B68">
-        <v>33000</v>
+        <v>26000</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68">
-        <v>32</v>
+        <v>6292</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -2694,16 +2710,16 @@
         <v>0</v>
       </c>
       <c r="G68">
-        <v>1935</v>
+        <v>0</v>
       </c>
       <c r="H68">
         <v>0</v>
       </c>
       <c r="I68">
-        <v>34967</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>32292</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -2711,39 +2727,39 @@
         <v>26000</v>
       </c>
       <c r="C69">
+        <v>2550</v>
+      </c>
+      <c r="D69">
         <v>828</v>
       </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
       <c r="E69">
-        <v>0</v>
+        <v>2769</v>
       </c>
       <c r="F69">
         <v>0</v>
       </c>
       <c r="G69">
-        <v>2776</v>
+        <v>0</v>
       </c>
       <c r="H69">
-        <v>2470</v>
+        <v>0</v>
       </c>
       <c r="I69">
-        <v>32074</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <v>32147</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>77</v>
       </c>
       <c r="B70">
-        <v>26000</v>
+        <v>27000</v>
       </c>
       <c r="C70">
-        <v>3270</v>
+        <v>102</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>3297</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -2755,21 +2771,21 @@
         <v>0</v>
       </c>
       <c r="H70">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="I70">
-        <v>29373</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+        <v>30399</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>78</v>
       </c>
       <c r="B71">
-        <v>21000</v>
+        <v>28000</v>
       </c>
       <c r="C71">
-        <v>6176</v>
+        <v>0</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -2787,15 +2803,15 @@
         <v>0</v>
       </c>
       <c r="I71">
-        <v>27176</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>79</v>
       </c>
       <c r="B72">
-        <v>27000</v>
+        <v>28000</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -2816,68 +2832,68 @@
         <v>0</v>
       </c>
       <c r="I72">
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>80</v>
       </c>
       <c r="B73">
-        <v>27000</v>
+        <v>20000</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>6810</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F73">
         <v>0</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H73">
         <v>0</v>
       </c>
       <c r="I73">
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
+        <v>26854</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>81</v>
       </c>
       <c r="B74">
-        <v>20000</v>
+        <v>24000</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>1140</v>
       </c>
       <c r="D74">
         <v>0</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>646</v>
       </c>
       <c r="F74">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G74">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H74">
-        <v>6400</v>
+        <v>0</v>
       </c>
       <c r="I74">
-        <v>26440</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
+        <v>25786</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -2885,7 +2901,7 @@
         <v>25000</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>518</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -2900,13 +2916,13 @@
         <v>0</v>
       </c>
       <c r="H75">
-        <v>504</v>
+        <v>0</v>
       </c>
       <c r="I75">
-        <v>25504</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
+        <v>25518</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -2935,12 +2951,12 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>84</v>
       </c>
       <c r="B77">
-        <v>23000</v>
+        <v>25000</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -2955,16 +2971,16 @@
         <v>0</v>
       </c>
       <c r="G77">
-        <v>655</v>
+        <v>0</v>
       </c>
       <c r="H77">
-        <v>1130</v>
+        <v>0</v>
       </c>
       <c r="I77">
-        <v>24785</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -2972,13 +2988,13 @@
         <v>23000</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="D78">
         <v>0</v>
       </c>
       <c r="E78">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -2987,42 +3003,42 @@
         <v>0</v>
       </c>
       <c r="H78">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="I78">
-        <v>23212</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
+        <v>23222</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>86</v>
       </c>
       <c r="B79">
-        <v>23000</v>
+        <v>21000</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>236</v>
       </c>
       <c r="D79">
         <v>0</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="F79">
         <v>0</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>1687</v>
       </c>
       <c r="H79">
         <v>0</v>
       </c>
       <c r="I79">
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
+        <v>23011</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -3051,12 +3067,12 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>88</v>
       </c>
       <c r="B81">
-        <v>18000</v>
+        <v>0</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -3068,19 +3084,19 @@
         <v>0</v>
       </c>
       <c r="F81">
-        <v>1429</v>
+        <v>0</v>
       </c>
       <c r="G81">
-        <v>87</v>
+        <v>21800</v>
       </c>
       <c r="H81">
-        <v>229</v>
+        <v>0</v>
       </c>
       <c r="I81">
-        <v>19745</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
+        <v>21800</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -3088,28 +3104,28 @@
         <v>14000</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>763</v>
       </c>
       <c r="D82">
         <v>0</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>2475</v>
       </c>
       <c r="F82">
         <v>0</v>
       </c>
       <c r="G82">
-        <v>2491</v>
+        <v>0</v>
       </c>
       <c r="H82">
-        <v>740</v>
+        <v>0</v>
       </c>
       <c r="I82">
-        <v>17231</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
+        <v>17238</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>90</v>
       </c>
@@ -3117,28 +3133,28 @@
         <v>0</v>
       </c>
       <c r="C83">
-        <v>7445</v>
+        <v>0</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>7460</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>4251</v>
       </c>
       <c r="F83">
-        <v>2772</v>
+        <v>0</v>
       </c>
       <c r="G83">
-        <v>4229</v>
+        <v>2943</v>
       </c>
       <c r="H83">
         <v>0</v>
       </c>
       <c r="I83">
-        <v>14446</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9">
+        <v>14654</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -3146,10 +3162,10 @@
         <v>9800</v>
       </c>
       <c r="C84">
-        <v>3036</v>
+        <v>0</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>3020</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -3164,27 +3180,27 @@
         <v>0</v>
       </c>
       <c r="I84">
-        <v>12836</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9">
+        <v>12820</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>92</v>
       </c>
       <c r="B85">
-        <v>7300</v>
+        <v>7500</v>
       </c>
       <c r="C85">
-        <v>3959</v>
+        <v>0</v>
       </c>
       <c r="D85">
-        <v>794</v>
+        <v>4207</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>803</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -3193,76 +3209,76 @@
         <v>0</v>
       </c>
       <c r="I85">
-        <v>12053</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
+        <v>12510</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>93</v>
       </c>
       <c r="B86">
-        <v>3800</v>
+        <v>3000</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>2440</v>
       </c>
       <c r="D86">
-        <v>7658</v>
+        <v>106</v>
       </c>
       <c r="E86">
         <v>0</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>6289</v>
       </c>
       <c r="G86">
         <v>0</v>
       </c>
       <c r="H86">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="I86">
-        <v>11533</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
+        <v>11835</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>94</v>
       </c>
       <c r="B87">
-        <v>3000</v>
+        <v>3900</v>
       </c>
       <c r="C87">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="D87">
-        <v>5991</v>
+        <v>0</v>
       </c>
       <c r="E87">
         <v>0</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>7819</v>
       </c>
       <c r="G87">
         <v>0</v>
       </c>
       <c r="H87">
-        <v>2310</v>
+        <v>0</v>
       </c>
       <c r="I87">
-        <v>11404</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9">
+        <v>11795</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>95</v>
       </c>
       <c r="B88">
-        <v>9500</v>
+        <v>10000</v>
       </c>
       <c r="C88">
-        <v>1418</v>
+        <v>0</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -3277,27 +3293,27 @@
         <v>0</v>
       </c>
       <c r="H88">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="I88">
-        <v>10918</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>96</v>
       </c>
       <c r="B89">
-        <v>9900</v>
+        <v>9500</v>
       </c>
       <c r="C89">
         <v>0</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>1454</v>
       </c>
       <c r="E89">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F89">
         <v>0</v>
@@ -3309,10 +3325,10 @@
         <v>0</v>
       </c>
       <c r="I89">
-        <v>10900</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
+        <v>10954</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -3320,28 +3336,28 @@
         <v>6800</v>
       </c>
       <c r="C90">
-        <v>1440</v>
+        <v>1110</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>894</v>
       </c>
       <c r="F90">
         <v>0</v>
       </c>
       <c r="G90">
-        <v>892</v>
+        <v>0</v>
       </c>
       <c r="H90">
-        <v>1090</v>
+        <v>0</v>
       </c>
       <c r="I90">
-        <v>10222</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
+        <v>10304</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -3349,28 +3365,28 @@
         <v>8100</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="D91">
-        <v>629</v>
+        <v>0</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="F91">
-        <v>700</v>
+        <v>642</v>
       </c>
       <c r="G91">
-        <v>42</v>
+        <v>718</v>
       </c>
       <c r="H91">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="I91">
-        <v>9555</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
+        <v>9590</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>99</v>
       </c>
@@ -3378,10 +3394,10 @@
         <v>7900</v>
       </c>
       <c r="C92">
-        <v>323</v>
+        <v>0</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>324</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -3396,21 +3412,21 @@
         <v>0</v>
       </c>
       <c r="I92">
-        <v>8223</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
+        <v>8224</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>100</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>6900</v>
       </c>
       <c r="C93">
         <v>0</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>1098</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -3419,30 +3435,30 @@
         <v>0</v>
       </c>
       <c r="G93">
-        <v>8076</v>
+        <v>0</v>
       </c>
       <c r="H93">
         <v>0</v>
       </c>
       <c r="I93">
-        <v>8076</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
+        <v>7998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>101</v>
       </c>
       <c r="B94">
-        <v>6800</v>
+        <v>6400</v>
       </c>
       <c r="C94">
-        <v>1096</v>
+        <v>0</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>191</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>931</v>
       </c>
       <c r="F94">
         <v>0</v>
@@ -3454,18 +3470,18 @@
         <v>0</v>
       </c>
       <c r="I94">
-        <v>7896</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
+        <v>7522</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>102</v>
       </c>
       <c r="B95">
-        <v>6400</v>
+        <v>0</v>
       </c>
       <c r="C95">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -3474,30 +3490,30 @@
         <v>0</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>7207</v>
       </c>
       <c r="G95">
-        <v>935</v>
+        <v>0</v>
       </c>
       <c r="H95">
         <v>0</v>
       </c>
       <c r="I95">
-        <v>7521</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9">
+        <v>7207</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>103</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>5800</v>
       </c>
       <c r="C96">
         <v>0</v>
       </c>
       <c r="D96">
-        <v>7189</v>
+        <v>0</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -3512,21 +3528,21 @@
         <v>0</v>
       </c>
       <c r="I96">
-        <v>7189</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>104</v>
       </c>
       <c r="B97">
-        <v>5800</v>
+        <v>5300</v>
       </c>
       <c r="C97">
         <v>0</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -3541,18 +3557,18 @@
         <v>0</v>
       </c>
       <c r="I97">
-        <v>5800</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
+        <v>5780</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>105</v>
       </c>
       <c r="B98">
-        <v>5200</v>
+        <v>1400</v>
       </c>
       <c r="C98">
-        <v>476</v>
+        <v>389</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -3561,7 +3577,7 @@
         <v>0</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>3620</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -3570,21 +3586,21 @@
         <v>0</v>
       </c>
       <c r="I98">
-        <v>5676</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
+        <v>5409</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>106</v>
       </c>
       <c r="B99">
-        <v>1400</v>
+        <v>3400</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="D99">
-        <v>3574</v>
+        <v>410</v>
       </c>
       <c r="E99">
         <v>0</v>
@@ -3596,24 +3612,24 @@
         <v>0</v>
       </c>
       <c r="H99">
-        <v>369</v>
+        <v>0</v>
       </c>
       <c r="I99">
-        <v>5343</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
+        <v>3848</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>107</v>
       </c>
       <c r="B100">
-        <v>3400</v>
+        <v>2100</v>
       </c>
       <c r="C100">
-        <v>401</v>
+        <v>0</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>1314</v>
       </c>
       <c r="E100">
         <v>0</v>
@@ -3625,24 +3641,24 @@
         <v>0</v>
       </c>
       <c r="H100">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="I100">
-        <v>3838</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
+        <v>3414</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>108</v>
       </c>
       <c r="B101">
-        <v>2100</v>
+        <v>2400</v>
       </c>
       <c r="C101">
-        <v>1312</v>
+        <v>0</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>808</v>
       </c>
       <c r="E101">
         <v>0</v>
@@ -3657,18 +3673,18 @@
         <v>0</v>
       </c>
       <c r="I101">
-        <v>3412</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9">
+        <v>3208</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>109</v>
       </c>
       <c r="B102">
-        <v>2400</v>
+        <v>2500</v>
       </c>
       <c r="C102">
-        <v>817</v>
+        <v>0</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -3686,15 +3702,15 @@
         <v>0</v>
       </c>
       <c r="I102">
-        <v>3217</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>110</v>
       </c>
       <c r="B103">
-        <v>2500</v>
+        <v>2300</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -3715,15 +3731,15 @@
         <v>0</v>
       </c>
       <c r="I103">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>111</v>
       </c>
       <c r="B104">
-        <v>2300</v>
+        <v>2200</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -3744,15 +3760,15 @@
         <v>0</v>
       </c>
       <c r="I104">
-        <v>2300</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>112</v>
       </c>
       <c r="B105">
-        <v>2200</v>
+        <v>2100</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -3773,18 +3789,18 @@
         <v>0</v>
       </c>
       <c r="I105">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>113</v>
       </c>
       <c r="B106">
-        <v>2100</v>
+        <v>1500</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -3802,15 +3818,15 @@
         <v>0</v>
       </c>
       <c r="I106">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>114</v>
       </c>
       <c r="B107">
-        <v>1400</v>
+        <v>0</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -3822,30 +3838,30 @@
         <v>0</v>
       </c>
       <c r="F107">
-        <v>0</v>
+        <v>1102</v>
       </c>
       <c r="G107">
         <v>0</v>
       </c>
       <c r="H107">
-        <v>314</v>
+        <v>0</v>
       </c>
       <c r="I107">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>115</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="C108">
         <v>0</v>
       </c>
       <c r="D108">
-        <v>1101</v>
+        <v>0</v>
       </c>
       <c r="E108">
         <v>0</v>
@@ -3860,65 +3876,7 @@
         <v>0</v>
       </c>
       <c r="I108">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9">
-      <c r="A109" t="s">
-        <v>116</v>
-      </c>
-      <c r="B109">
         <v>1000</v>
-      </c>
-      <c r="C109">
-        <v>0</v>
-      </c>
-      <c r="D109">
-        <v>0</v>
-      </c>
-      <c r="E109">
-        <v>0</v>
-      </c>
-      <c r="F109">
-        <v>0</v>
-      </c>
-      <c r="G109">
-        <v>0</v>
-      </c>
-      <c r="H109">
-        <v>0</v>
-      </c>
-      <c r="I109">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9">
-      <c r="A110" t="s">
-        <v>117</v>
-      </c>
-      <c r="B110">
-        <v>0</v>
-      </c>
-      <c r="C110">
-        <v>0</v>
-      </c>
-      <c r="D110">
-        <v>0</v>
-      </c>
-      <c r="E110">
-        <v>0</v>
-      </c>
-      <c r="F110">
-        <v>0</v>
-      </c>
-      <c r="G110">
-        <v>660</v>
-      </c>
-      <c r="H110">
-        <v>54</v>
-      </c>
-      <c r="I110">
-        <v>714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>